<commit_message>
[IMP] Adjust CD Receivable Confirmation Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_confirmation.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_confirmation.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Confirmation Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Confirmation Detail Report" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Receivable CD Confirmation Detail Report" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -71,7 +71,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
@@ -212,6 +212,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -362,6 +374,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:G1048576">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Total",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
[IMP] Adjust CD Receivable Confirmation
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_confirmation.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_confirmation.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Confirmation Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Confirmation Detail Report" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,18 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Receivable CD Confirmation Report</t>
   </si>
   <si>
-    <t xml:space="preserve">Report Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank</t>
+    <t xml:space="preserve">Customer CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer (bank)</t>
   </si>
   <si>
     <t xml:space="preserve">Run By</t>
@@ -60,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">Outstanding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice</t>
   </si>
 </sst>
 </file>
@@ -187,14 +180,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,12 +198,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -292,7 +285,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -329,13 +322,13 @@
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -343,34 +336,28 @@
       </c>
       <c r="B6" s="8"/>
     </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -387,105 +374,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="35.58"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="3" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>